<commit_message>
Fixing import export Excel.
</commit_message>
<xml_diff>
--- a/GEAK_Testobjekt_Meier.xlsx
+++ b/GEAK_Testobjekt_Meier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taamepar/dev/experiments/geak4s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8009_{1D304D25-FC4E-5C44-9890-74B50A0611C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8009_{F15F1AB4-1BEB-9B4A-8CED-CA10852FDF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" tabRatio="906" xr2:uid="{2DA48115-A043-C244-944E-500FBFD6D879}"/>
@@ -2214,7 +2214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1198" uniqueCount="812">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1200" uniqueCount="814">
   <si>
     <t>Projektbezeichnung</t>
   </si>
@@ -4650,6 +4650,12 @@
   </si>
   <si>
     <t>Ölheizung</t>
+  </si>
+  <si>
+    <t>Breite 4</t>
+  </si>
+  <si>
+    <t>6487 Göschenen</t>
   </si>
 </sst>
 </file>
@@ -7727,7 +7733,7 @@
             <xdr:cNvPr id="1025" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F205612-AD31-E144-8403-D58BD6B1486A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFEE90AC-21F6-8A27-E0B7-04149EBBF0A9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7825,7 +7831,7 @@
             <xdr:cNvPr id="1026" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE0801C-7211-AF22-2987-4A6C1FDAD131}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79C650E-DE1B-30CF-F334-34269E30EE3D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7928,7 +7934,7 @@
             <xdr:cNvPr id="10241" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C2F0D9-906D-3318-EE93-C8AF86C3DFCE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD9E452-610B-CA40-E055-29DB2CD18B94}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8026,7 +8032,7 @@
             <xdr:cNvPr id="10242" name="Comment 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E8E5A4-F163-CFE9-2F4F-FDEBC3354C4A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3102B984-516E-8E90-752E-B55FE8FF5977}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8124,7 +8130,7 @@
             <xdr:cNvPr id="10243" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA243871-F56E-3DB5-FD34-062721F23548}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D649A19F-AE98-7088-7F98-438E31587931}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8234,7 +8240,7 @@
             <xdr:cNvPr id="10244" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E47FAC3E-C9B7-057E-110E-A00C14DCB50E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541EE64F-2F98-7376-8EB3-E3F553A4D230}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8337,7 +8343,7 @@
             <xdr:cNvPr id="11265" name="Comment 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F561A1F-A285-A6F8-8CAA-5B405780486A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02AAE93C-82D8-B42E-842A-72A4B126F90E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8435,7 +8441,7 @@
             <xdr:cNvPr id="11266" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B11DA232-DA58-1293-459B-5D369F8521C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D496BB51-351B-55A7-111D-890081BA4643}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8545,7 +8551,7 @@
             <xdr:cNvPr id="11267" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2410A9C5-0923-E558-A83D-94B36E6DA932}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1DBEC4-88A0-95F9-F25A-B4DE2A2999B8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8648,7 +8654,7 @@
             <xdr:cNvPr id="12289" name="Comment 1027">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B1D1ED-1086-5474-398C-6258A5477D0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186DAE03-0D19-4B34-714C-4EA583E72260}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8751,7 +8757,7 @@
             <xdr:cNvPr id="12290" name="Comment 1029">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEF4954-3119-F8B9-6E6A-D6F0BBB0F470}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDF167C-3386-311E-5C55-174F7DE062BA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8854,7 +8860,7 @@
             <xdr:cNvPr id="13313" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94838C23-C2FF-E200-8E9D-A3040AD1F0AA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA9369B8-1D67-7F9A-EEED-5E2791304B7D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8952,7 +8958,7 @@
             <xdr:cNvPr id="13314" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE23BA8D-B0DB-99E4-E99B-43322D4991C1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E53B59-D576-C872-1B29-42ABFB0E9639}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9050,7 +9056,7 @@
             <xdr:cNvPr id="13315" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B866386-314D-D94C-5FE3-8CB5788D0F07}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C08791-24A3-E583-A397-7CEFBD2048F4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9165,7 +9171,7 @@
             <xdr:cNvPr id="14337" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10DBCA22-DCA8-E5B2-0BDA-16CFC1A0D02F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{727787F4-BD17-2D99-404E-39EC95DA0093}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9263,7 +9269,7 @@
             <xdr:cNvPr id="14338" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFBF5D5B-C8F3-FFA1-7230-EAC3CEAFD8D2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5779DE09-D029-8ACF-017A-B32AF016F358}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9361,7 +9367,7 @@
             <xdr:cNvPr id="14339" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7747C993-D097-D32F-CC86-0FE8F5A61103}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16BFBBEF-7702-4185-4273-4DBABB8339FC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9464,7 +9470,7 @@
             <xdr:cNvPr id="15361" name="Comment 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E08FBB4-D80C-D794-1D65-C9C27D5B3B4F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A186A566-F218-18AB-05C9-55D33470F38F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9562,7 +9568,7 @@
             <xdr:cNvPr id="15362" name="Comment 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668E0215-80A9-3341-6ABE-2F1EFED89638}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D04E46-6595-C542-7BD4-5E466907E445}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9665,7 +9671,7 @@
             <xdr:cNvPr id="16385" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B96987-5CAE-6A55-A446-5DDCF09F1A76}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5278DF7-8F8D-24F7-FF9D-712241FE0343}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9763,7 +9769,7 @@
             <xdr:cNvPr id="16386" name="Comment 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25180FA9-99A7-00AF-BE32-D3A9D38BD1F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF484BC6-39F6-9CDF-5877-F0A2F66E6813}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9851,7 +9857,7 @@
             <xdr:cNvPr id="16387" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765FFD49-C349-C5FD-8F07-836DE856A1B0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92DF4A82-9207-2434-5053-A74DB8120BCB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9954,7 +9960,7 @@
             <xdr:cNvPr id="2049" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B421E18-004C-8D73-CC81-614B3197CEE7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85AD79FD-0AC5-E898-D086-DB45E2B0FF9F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10052,7 +10058,7 @@
             <xdr:cNvPr id="2050" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC00FE33-A177-D502-74F5-AC8F03F319D7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{589B2382-25CB-93C9-D058-DC61B7C2EE3D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10155,7 +10161,7 @@
             <xdr:cNvPr id="3073" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{804A46FD-9309-1B91-871E-D75C977D10ED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17644E1D-1076-9222-E923-2EB143C50190}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10253,7 +10259,7 @@
             <xdr:cNvPr id="3074" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A0F461C-E61C-622E-BB15-7A8D1790F1F2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28CF2A31-55D3-3606-2AFA-3CA69AE020A3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10363,7 +10369,7 @@
             <xdr:cNvPr id="3075" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2E0DD4-FB7A-534C-8F71-128EB762AC4A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8137A40B-A05A-DF50-983E-D29B3178FB85}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10466,7 +10472,7 @@
             <xdr:cNvPr id="4097" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22ACB44C-407B-44B1-2560-87746EE155F9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948ADFA0-871F-2BDE-5A25-1EE66BBDBEB3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10564,7 +10570,7 @@
             <xdr:cNvPr id="4098" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FA677BF-C1E5-92BA-CC66-3DAC19AF4C4E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F29DE71-F4CA-5BA3-5445-FC79D630F774}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10667,7 +10673,7 @@
             <xdr:cNvPr id="5121" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{962533BC-221A-A469-993F-BA088A1C3F62}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4B37A7E-5A2E-DAB6-7E86-259F96DF1BAA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10765,7 +10771,7 @@
             <xdr:cNvPr id="5122" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48907B01-6A8F-CABE-54F2-B62C6F58BCA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C44CB3CF-FE65-8EA6-F530-EB24D5E2794D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10868,7 +10874,7 @@
             <xdr:cNvPr id="6145" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CD58B2A-2BAC-CF44-EB2A-E88BA92B76F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D4381B6-533A-B929-F46A-8D59C1E05A10}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10971,7 +10977,7 @@
             <xdr:cNvPr id="7169" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5073A1F5-5F9C-2009-97E3-7E3B5EA00FC9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF44A5B0-F42B-C10F-39FF-A8298F0AB732}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11069,7 +11075,7 @@
             <xdr:cNvPr id="7170" name="Comment 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEC02279-7AB1-F1C1-F43D-4D6B09AF7D47}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097AA1DB-0C54-0716-522F-379CF84A207A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11172,7 +11178,7 @@
             <xdr:cNvPr id="8193" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E869D068-CE07-B9DC-C475-054F4D51D4FA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EAEE745-7BBC-6C75-CD7D-C695A9D186F0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11270,7 +11276,7 @@
             <xdr:cNvPr id="8194" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{077E1976-2422-7571-6BB4-DCE76E31E7AD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E472C20C-BE31-E425-2760-8C04F7E6EA8D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11373,7 +11379,7 @@
             <xdr:cNvPr id="9217" name="Comment 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66835154-7662-A980-30AF-27BF02A1E8C4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F73FF1-266F-4C7C-FD6C-7E2C6B541A62}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11476,7 +11482,7 @@
             <xdr:cNvPr id="9218" name="Comment 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9742195F-A236-6FB6-D60B-9EF510F52C32}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC434586-53F0-32B1-A4C1-CB3D37EBC9FE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11574,7 +11580,7 @@
             <xdr:cNvPr id="9219" name="Comment 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAEBC899-9153-1FF9-8A46-E4D14B16CF0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3AE3C6-53CB-F134-DBDF-71F92690E8B4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12045,7 +12051,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12127,6 +12133,18 @@
       </c>
       <c r="B6" s="12" t="s">
         <v>797</v>
+      </c>
+      <c r="D6" s="9">
+        <v>123434</v>
+      </c>
+      <c r="E6" s="9">
+        <v>23423</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>